<commit_message>
[Update] Implement API for date picker
</commit_message>
<xml_diff>
--- a/response_api.xlsx
+++ b/response_api.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web_App\Michael\Sapient\Sapient\Energy-Chatbot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web_App\Michael\Sapient\Energy-Chatbot-Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AEABEA8-67AF-45A9-88D9-50D9D0E60D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CF78C3-91D8-442B-AF62-407EFB9413FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>Response</t>
   </si>
@@ -118,13 +118,16 @@
   </si>
   <si>
     <t>Return top 5 contributors (specific pieces of equipment) that contributed to a change in energy consumption for [a specific space type]</t>
+  </si>
+  <si>
+    <t>Format</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,12 +155,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -179,14 +176,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,219 +465,296 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="94.85546875" customWidth="1"/>
-    <col min="2" max="2" width="63.85546875" customWidth="1"/>
+    <col min="1" max="1" width="111.7109375" customWidth="1"/>
+    <col min="2" max="2" width="63.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Update] Implement changing function buttons to short description for button
</commit_message>
<xml_diff>
--- a/response_api.xlsx
+++ b/response_api.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web_App\Michael\Sapient\Energy-Chatbot-Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D6B0189-44FE-4CB7-A32E-630BE0310BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAC7134-4E5A-4E5E-96C4-D359931ED069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="23310" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
   <si>
     <t>Response</t>
   </si>
@@ -124,6 +124,33 @@
   </si>
   <si>
     <t>Title</t>
+  </si>
+  <si>
+    <t>See my after hours energy consumption sorted by end use</t>
+  </si>
+  <si>
+    <t>Compare my after hours energy consumption to my total energy consumption</t>
+  </si>
+  <si>
+    <t>See my total energy consumption</t>
+  </si>
+  <si>
+    <t>See my total energy consumption and end use breakdown</t>
+  </si>
+  <si>
+    <t>See my total energy consumption for a specific end use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tell me how much energy was used by a specific piece of equipment </t>
+  </si>
+  <si>
+    <t>Identify the maximum power draw and time it happened for a piece of equipment</t>
+  </si>
+  <si>
+    <t>Identify the maximum energy consumption and the approximate time it occured in my building</t>
+  </si>
+  <si>
+    <t>See my monthly energy consumption (see, look at, inspect, compare, analyze: Verb + what they want to do)</t>
   </si>
 </sst>
 </file>
@@ -470,23 +497,23 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" customWidth="1"/>
-    <col min="2" max="2" width="111.7109375" customWidth="1"/>
+    <col min="1" max="1" width="111.7109375" customWidth="1"/>
+    <col min="2" max="2" width="56" customWidth="1"/>
     <col min="3" max="3" width="63.85546875" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -496,9 +523,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -507,8 +535,11 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -518,8 +549,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -529,8 +563,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>8</v>
@@ -540,8 +577,11 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="A6" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>6</v>
@@ -551,8 +591,11 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>6</v>
@@ -562,8 +605,11 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>12</v>
@@ -573,9 +619,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
@@ -584,9 +631,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
         <v>14</v>
       </c>
@@ -595,9 +643,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="B11" s="3"/>
       <c r="C11" s="4" t="s">
         <v>3</v>
       </c>
@@ -606,8 +655,11 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="B12" s="3" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>6</v>
@@ -617,8 +669,11 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="3" t="s">
         <v>17</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -628,8 +683,11 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>12</v>
@@ -639,8 +697,11 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>20</v>
@@ -650,8 +711,11 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="3" t="s">
         <v>21</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>8</v>
@@ -660,10 +724,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="B17" s="3"/>
       <c r="C17" s="4" t="s">
         <v>8</v>
       </c>
@@ -671,10 +736,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="B18" s="3"/>
       <c r="C18" t="s">
         <v>6</v>
       </c>
@@ -682,10 +748,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="B19" s="3"/>
       <c r="C19" s="4" t="s">
         <v>3</v>
       </c>
@@ -693,10 +760,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="B20" s="3"/>
       <c r="C20" t="s">
         <v>6</v>
       </c>
@@ -704,10 +772,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="B21" s="3"/>
       <c r="C21" s="4" t="s">
         <v>12</v>
       </c>
@@ -715,10 +784,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="B22" s="3"/>
       <c r="C22" s="4" t="s">
         <v>14</v>
       </c>
@@ -726,10 +796,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="B23" s="3"/>
       <c r="C23" s="4" t="s">
         <v>14</v>
       </c>
@@ -737,10 +808,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="B24" s="3"/>
       <c r="C24" s="4" t="s">
         <v>14</v>
       </c>
@@ -748,10 +820,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="B25" s="3"/>
       <c r="C25" s="4" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
[Update] Implementing dropdown feature
</commit_message>
<xml_diff>
--- a/response_api.xlsx
+++ b/response_api.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web_App\Michael\Sapient\Energy-Chatbot-Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAC7134-4E5A-4E5E-96C4-D359931ED069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FB2E08-FF60-4F30-B278-07C502320814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t>Response</t>
   </si>
@@ -151,6 +151,15 @@
   </si>
   <si>
     <t>See my monthly energy consumption (see, look at, inspect, compare, analyze: Verb + what they want to do)</t>
+  </si>
+  <si>
+    <t>Dropdown</t>
+  </si>
+  <si>
+    <t>end_use</t>
+  </si>
+  <si>
+    <t>equipment</t>
   </si>
 </sst>
 </file>
@@ -494,21 +503,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="111.7109375" customWidth="1"/>
-    <col min="2" max="2" width="56" customWidth="1"/>
+    <col min="1" max="1" width="94.42578125" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" customWidth="1"/>
     <col min="3" max="3" width="63.85546875" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -521,8 +531,11 @@
       <c r="D1" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -534,7 +547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -548,7 +561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -562,7 +575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -576,7 +589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -590,7 +603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -603,8 +616,11 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -617,8 +633,11 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -630,7 +649,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -642,7 +661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -654,7 +673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
@@ -668,7 +687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
@@ -682,7 +701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -695,8 +714,11 @@
       <c r="D14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>19</v>
       </c>
@@ -710,7 +732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
[Update] Modified monster content answer part & Added start prompt generating
</commit_message>
<xml_diff>
--- a/response_api.xlsx
+++ b/response_api.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web_App\Michael\Sapient\Energy-Chatbot-Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FB2E08-FF60-4F30-B278-07C502320814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A3E137-891F-4883-A883-80D8B9666A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="23310" windowHeight="13740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart2" sheetId="3" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="45">
   <si>
     <t>Response</t>
   </si>
@@ -238,6 +240,2046 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$25:$C$25</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Return top 5 contributors (specific pieces of equipment) that contributed to a change in energy consumption for [a specific space type]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>get_explorer_equip_power_consumption</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$D$1:$E$24</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>equipment</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>end_use</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>equipment</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>end_use</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>equipment</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>end_use</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>4</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>equipment</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>end_use</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>equipment</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>end_use</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>equipment</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>end_use</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>end_use</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>3</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Format</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dropdown</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$25:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1CBB-4B87-BF23-BBD188D923FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="757401711"/>
+        <c:axId val="676569199"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="757401711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="676569199"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="676569199"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="757401711"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$25:$C$25</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Return top 5 contributors (specific pieces of equipment) that contributed to a change in energy consumption for [a specific space type]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>get_explorer_equip_power_consumption</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$D$1:$E$24</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>equipment</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>end_use</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>equipment</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>end_use</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>equipment</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>end_use</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>4</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>equipment</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>end_use</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>equipment</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>end_use</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>equipment</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>end_use</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>end_use</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>3</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Format</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Dropdown</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$25:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-118E-4D99-A048-030226D8850F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="671972431"/>
+        <c:axId val="678244463"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="671972431"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="678244463"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="678244463"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="671972431"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{7C8569EA-9CBB-43EC-8D59-88EE04DA15EE}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{ABA5B5B6-C237-4880-9BBB-9472948EA943}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="123" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8673171" cy="6295793"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BE090A0-7DC2-FAEB-74DF-CBA655148095}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8673171" cy="6295793"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3475A0D1-587C-AE5A-2C9B-9D8F828D9A78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -505,16 +2547,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="94.42578125" customWidth="1"/>
+    <col min="1" max="1" width="78.7109375" customWidth="1"/>
     <col min="2" max="2" width="46.28515625" customWidth="1"/>
     <col min="3" max="3" width="63.85546875" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
     <col min="5" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -602,6 +2644,9 @@
       <c r="D6">
         <v>3</v>
       </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -648,6 +2693,9 @@
       <c r="D9">
         <v>2</v>
       </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -660,6 +2708,9 @@
       <c r="D10">
         <v>2</v>
       </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -700,6 +2751,9 @@
       <c r="D13">
         <v>1</v>
       </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -746,7 +2800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
@@ -758,7 +2812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>23</v>
       </c>
@@ -769,8 +2823,11 @@
       <c r="D18">
         <v>2</v>
       </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
@@ -781,8 +2838,11 @@
       <c r="D19">
         <v>2</v>
       </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>25</v>
       </c>
@@ -793,8 +2853,11 @@
       <c r="D20">
         <v>1</v>
       </c>
+      <c r="E20" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
@@ -805,8 +2868,11 @@
       <c r="D21">
         <v>1</v>
       </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
@@ -818,7 +2884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
@@ -829,8 +2895,11 @@
       <c r="D23">
         <v>2</v>
       </c>
+      <c r="E23" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
@@ -841,8 +2910,11 @@
       <c r="D24">
         <v>2</v>
       </c>
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>30</v>
       </c>

</xml_diff>